<commit_message>
feat: Implement Local LLM for Q&A, replacing Excel-based system
- Added LocalLLMDatabase class to handle queries using a local LLM via Ollama.
- Integrated wakeword detection and conversation management.
- Implemented TTS using Piper for audio responses.
- Enhanced state management for conversation flow and user interaction.
- Developed Flask web UI for real-time status updates and interaction.
- Included face recognition for personalized greetings.
- Added Hindi wakeword detection for multilingual support.
</commit_message>
<xml_diff>
--- a/qa_database.xlsx
+++ b/qa_database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -622,6 +622,168 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>What are the college's admission criteria?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>The college's admission criteria include academic performance, entrance exam scores, and extracurricular activities.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>कॉलेज के प्रवेश मानदंड क्या हैं?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>कॉलेज के प्रवेश मानदंडों में शैक्षणिक प्रदर्शन, प्रवेश परीक्षा के अंक, और सह-पाठ्यक्रम गतिविधियाँ शामिल हैं।</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>admission criteria, college, academic performance, entrance exam</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>What facilities are available on campus?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>The campus offers facilities such as a library, sports complex, canteen, and hostels.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>कैंपस में कौन-कौन सी सुविधाएँ उपलब्ध हैं?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>कैंपस में पुस्तकालय, खेल परिसर, कैफेटेरिया, और हॉस्टल जैसी सुविधाएँ उपलब्ध हैं।</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>facilities, campus, library, sports complex, cafeteria, hostels</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>What extracurricular activities does the college offer?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>The college offers various extracurricular activities including sports, cultural events, and technical workshops.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>कॉलेज कौन-कौन सी सह-पाठ्यक्रम गतिविधियाँ ऑफर करता है?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>कॉलेज विभिन्न सह-पाठ्यक्रम गतिविधियाँ ऑफर करता है जिनमें खेल, सांस्कृतिक कार्यक्रम, और तकनीकी कार्यशालाएँ शामिल हैं।</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>extracurricular activities, college, sports, cultural events, technical clubs</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>How can I contact the college administration?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>You can contact the college administration via phone, email, or by visiting the administrative office on campus.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>मैं कॉलेज प्रशासन से कैसे संपर्क कर सकता हूँ?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>आप फोन, ईमेल के माध्यम से या कैंपस में प्रशासनिक कार्यालय का दौरा करके कॉलेज प्रशासन से संपर्क कर सकते हैं।</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>contact, college administration, phone, email, office</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Who is the addmission incharge of the college</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>The admission incharge of the college is Mr. Atul Chakrawarti.</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>कॉलेज के एडमिशन इंचार्ज कौन हैं?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>कॉलेज के एडमिशन इंचार्ज श्री अतुल चक्रवर्ती हैं।</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>admission incharge, college, Mr. Atul Chakrawarti</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>What is the location of the college?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>The college is located in Raipur, Chhattisgarh, India.</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>कॉलेज का स्थान क्या है?</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>कॉलेज रायपुर, छत्तीसगढ़, भारत में स्थित है।</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>location, college, Raipur, Chhattisgarh</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>